<commit_message>
made a display for sets
</commit_message>
<xml_diff>
--- a/WebAplicationTestMVCSOL/WebAplicationTestMVC/Data/data.xlsx
+++ b/WebAplicationTestMVCSOL/WebAplicationTestMVC/Data/data.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,41 +22,40 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t xml:space="preserve">ID</t>
+    <t>ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Question</t>
+    <t>Question</t>
   </si>
   <si>
-    <t xml:space="preserve">Answer</t>
+    <t>Answer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="12">
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="186"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="186"/>
     </font>
     <font>
       <sz val="10"/>
@@ -74,7 +73,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalUp="1" diagonalDown="1">
       <left/>
       <right/>
       <top/>
@@ -82,48 +81,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="6">
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" borderId="0" applyBorder="1" applyProtection="1" applyAlignment="1"/>
+    <xf numFmtId="43" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
+    <xf numFmtId="41" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
+    <xf numFmtId="44" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
+    <xf numFmtId="42" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
+    <xf numFmtId="9" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -133,7 +109,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1048576"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -141,7 +117,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -152,14 +128,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" ht="12.8"/>
+    <row r="1048570" ht="12.8"/>
+    <row r="1048571" ht="12.8"/>
+    <row r="1048572" ht="12.8"/>
+    <row r="1048573" ht="12.8"/>
+    <row r="1048574" ht="12.8"/>
+    <row r="1048575" ht="12.8"/>
+    <row r="1048576" ht="12.8"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>